<commit_message>
update source code to fix bug: cannot restart ScheduleViewActivity
</commit_message>
<xml_diff>
--- a/documents/Plan/DetailPlan_LinhLLL.xlsx
+++ b/documents/Plan/DetailPlan_LinhLLL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15525" windowHeight="8235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10395"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="199">
   <si>
     <t>Task Name</t>
   </si>
@@ -327,18 +327,12 @@
     <t xml:space="preserve">       3.2.7.1 Use case diagram</t>
   </si>
   <si>
-    <t xml:space="preserve">       3.2.7.2 Report 1 (Draff)</t>
-  </si>
-  <si>
     <t xml:space="preserve">       3.2.7.3 System design</t>
   </si>
   <si>
     <t xml:space="preserve">       3.2.7.4 Database design</t>
   </si>
   <si>
-    <t xml:space="preserve">       3.2.7.4 Final GUI(Draff)</t>
-  </si>
-  <si>
     <t xml:space="preserve">       3.2.7.5 Schedule funtion ( Input screen)</t>
   </si>
   <si>
@@ -453,9 +447,6 @@
     <t>3.3 Sprint 2 ( Income and Expense management)</t>
   </si>
   <si>
-    <t xml:space="preserve">     3.3.2 Create GUI of Income and Expense management screen (Draff)</t>
-  </si>
-  <si>
     <t xml:space="preserve">     3.2.22 Review Schedule, Borrowing and Lending function</t>
   </si>
   <si>
@@ -607,6 +598,21 @@
   </si>
   <si>
     <t xml:space="preserve">         3.3.2.3 Warning screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     3.3.4  Update Report 2 (plan)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       3.3.7.1 Report 2 (ver 0.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     3.3.2 Create GUI of Income and Expense management screen (ver 0.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       3.2.7.2 Report 1 (ver 0.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       3.2.7.4 Final GUI(ver 0.1)</t>
   </si>
 </sst>
 </file>
@@ -1212,13 +1218,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.28515625" customWidth="1"/>
+    <col min="1" max="1" width="67" customWidth="1"/>
     <col min="2" max="6" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1729,7 +1735,7 @@
       </c>
       <c r="E30" s="24"/>
       <c r="F30" s="23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1747,7 +1753,7 @@
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1765,7 +1771,7 @@
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1783,7 +1789,7 @@
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1801,7 +1807,7 @@
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2085,12 +2091,12 @@
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>103</v>
+        <v>197</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>78</v>
@@ -2103,12 +2109,12 @@
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>78</v>
@@ -2121,12 +2127,12 @@
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>78</v>
@@ -2139,12 +2145,12 @@
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>106</v>
+        <v>198</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>78</v>
@@ -2157,12 +2163,12 @@
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>78</v>
@@ -2175,12 +2181,12 @@
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>78</v>
@@ -2193,12 +2199,12 @@
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>26</v>
@@ -2207,7 +2213,7 @@
         <v>79</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="2" t="s">
@@ -2216,7 +2222,7 @@
     </row>
     <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>26</v>
@@ -2225,7 +2231,7 @@
         <v>79</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2" t="s">
@@ -2234,7 +2240,7 @@
     </row>
     <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>26</v>
@@ -2243,7 +2249,7 @@
         <v>79</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2" t="s">
@@ -2252,7 +2258,7 @@
     </row>
     <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>26</v>
@@ -2261,14 +2267,14 @@
         <v>79</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>26</v>
@@ -2277,7 +2283,7 @@
         <v>79</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2" t="s">
@@ -2286,7 +2292,7 @@
     </row>
     <row r="63" spans="1:6" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>26</v>
@@ -2295,7 +2301,7 @@
         <v>79</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1" t="s">
@@ -2304,7 +2310,7 @@
     </row>
     <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>26</v>
@@ -2313,7 +2319,7 @@
         <v>79</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="2" t="s">
@@ -2322,7 +2328,7 @@
     </row>
     <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>26</v>
@@ -2331,7 +2337,7 @@
         <v>79</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="2" t="s">
@@ -2340,7 +2346,7 @@
     </row>
     <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>26</v>
@@ -2349,14 +2355,14 @@
         <v>79</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="2"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>22</v>
@@ -2365,7 +2371,7 @@
         <v>79</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2" t="s">
@@ -2374,16 +2380,16 @@
     </row>
     <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="2" t="s">
@@ -2392,7 +2398,7 @@
     </row>
     <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>22</v>
@@ -2401,7 +2407,7 @@
         <v>79</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="2" t="s">
@@ -2410,16 +2416,16 @@
     </row>
     <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="2" t="s">
@@ -2428,7 +2434,7 @@
     </row>
     <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2438,34 +2444,34 @@
     </row>
     <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="2" t="s">
@@ -2474,32 +2480,32 @@
     </row>
     <row r="74" spans="1:6" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
     </row>
     <row r="75" spans="1:6" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
@@ -2508,16 +2514,16 @@
     </row>
     <row r="76" spans="1:6" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1" t="s">
@@ -2526,16 +2532,16 @@
     </row>
     <row r="77" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="2" t="s">
@@ -2544,16 +2550,16 @@
     </row>
     <row r="78" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="2" t="s">
@@ -2562,34 +2568,34 @@
     </row>
     <row r="79" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2" t="s">
@@ -2598,16 +2604,16 @@
     </row>
     <row r="81" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E81" s="2"/>
       <c r="F81" s="2" t="s">
@@ -2616,7 +2622,7 @@
     </row>
     <row r="82" spans="1:6" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>21</v>
@@ -2629,12 +2635,12 @@
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="83" spans="1:6" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>21</v>
@@ -2650,64 +2656,64 @@
     </row>
     <row r="84" spans="1:6" s="27" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="23" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B84" s="23" t="s">
         <v>78</v>
       </c>
       <c r="C84" s="23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D84" s="23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E84" s="24"/>
       <c r="F84" s="24"/>
     </row>
     <row r="85" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="2"/>
     </row>
     <row r="86" spans="1:6" s="26" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B86" s="19" t="s">
         <v>18</v>
       </c>
       <c r="C86" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D86" s="19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E86" s="19"/>
       <c r="F86" s="19"/>
     </row>
     <row r="87" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" s="2" t="s">
@@ -2716,16 +2722,16 @@
     </row>
     <row r="88" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>145</v>
+        <v>196</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="2" t="s">
@@ -2734,16 +2740,16 @@
     </row>
     <row r="89" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" s="2" t="s">
@@ -2752,16 +2758,16 @@
     </row>
     <row r="90" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2" t="s">
@@ -2770,16 +2776,16 @@
     </row>
     <row r="91" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2" t="s">
@@ -2788,16 +2794,16 @@
     </row>
     <row r="92" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92" s="2" t="s">
@@ -2806,16 +2812,16 @@
     </row>
     <row r="93" spans="1:6" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="2" t="s">
@@ -2824,16 +2830,16 @@
     </row>
     <row r="94" spans="1:6" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="2" t="s">
@@ -2842,34 +2848,34 @@
     </row>
     <row r="95" spans="1:6" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="96" spans="1:6" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1" t="s">
@@ -2878,16 +2884,16 @@
     </row>
     <row r="97" spans="1:6" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1" t="s">
@@ -2896,122 +2902,122 @@
     </row>
     <row r="98" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C98" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D98" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B99" s="2" t="s">
+    <row r="99" spans="1:6" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A99" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="B99" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C99" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E99" s="2"/>
-      <c r="F99" s="2" t="s">
-        <v>135</v>
+      <c r="C99" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="D99" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="E99" s="23"/>
+      <c r="F99" s="23" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>167</v>
+        <v>195</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
     </row>
     <row r="104" spans="1:6" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C104" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D104" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1" t="s">
@@ -3020,34 +3026,34 @@
     </row>
     <row r="105" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="2" t="s">
@@ -3056,59 +3062,59 @@
     </row>
     <row r="107" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E108" s="2"/>
       <c r="F108" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="109" spans="1:6" s="26" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B109" s="19" t="s">
         <v>18</v>
       </c>
       <c r="C109" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D109" s="19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E109" s="19"/>
       <c r="F109" s="19"/>
     </row>
     <row r="110" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -3118,7 +3124,7 @@
     </row>
     <row r="111" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -3128,7 +3134,7 @@
     </row>
     <row r="112" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -3138,7 +3144,7 @@
     </row>
     <row r="113" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="28" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B113" s="28"/>
       <c r="C113" s="28"/>
@@ -3148,7 +3154,7 @@
     </row>
     <row r="114" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -3182,7 +3188,7 @@
     </row>
     <row r="115" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -3216,7 +3222,7 @@
     </row>
     <row r="116" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -3250,7 +3256,7 @@
     </row>
     <row r="117" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -3284,7 +3290,7 @@
     </row>
     <row r="118" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -3318,82 +3324,82 @@
     </row>
     <row r="119" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="29" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="120" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="121" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>153</v>
+        <v>194</v>
       </c>
     </row>
     <row r="122" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="123" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="124" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="125" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="126" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A126" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="126" spans="1:30" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A126" s="23" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="127" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="128" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>